<commit_message>
add main function call in eee_score.py
</commit_message>
<xml_diff>
--- a/files/第7期训练营11月评分.xlsx
+++ b/files/第7期训练营11月评分.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deronlee/PycharmProjects/EEEScoreCount/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4FD70C-BFF8-3C49-AC94-5689F9E15FBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14083006-D8E0-C445-816F-C8803E1E1E53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="1240" windowWidth="20500" windowHeight="13240" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="平时分" sheetId="1" r:id="rId1"/>
@@ -184,16 +184,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -485,13 +485,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
@@ -715,13 +715,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="16">
       <c r="A2" s="3" t="s">
@@ -936,7 +936,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F3" sqref="F3:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -961,16 +961,16 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -992,7 +992,7 @@
         <v>21.23</v>
       </c>
       <c r="F3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16">
@@ -1013,7 +1013,7 @@
         <v>20.91</v>
       </c>
       <c r="F4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16">
@@ -1034,7 +1034,7 @@
         <v>20.190000000000001</v>
       </c>
       <c r="F5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16">
@@ -1055,7 +1055,7 @@
         <v>18.759999999999998</v>
       </c>
       <c r="F6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16">
@@ -1076,7 +1076,7 @@
         <v>14.21</v>
       </c>
       <c r="F7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16">
@@ -1097,7 +1097,7 @@
         <v>13.51</v>
       </c>
       <c r="F8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16">
@@ -1118,7 +1118,7 @@
         <v>10.17</v>
       </c>
       <c r="F9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16">
@@ -1139,7 +1139,7 @@
         <v>10.11</v>
       </c>
       <c r="F10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16">
@@ -1160,7 +1160,7 @@
         <v>7.6300000000000008</v>
       </c>
       <c r="F11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16">
@@ -1181,7 +1181,7 @@
         <v>4.05</v>
       </c>
       <c r="F12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>